<commit_message>
Big commit - Trading plus Volatility and Timing Measures
</commit_message>
<xml_diff>
--- a/data/Triangular_Arbitrage_Binance.xlsx
+++ b/data/Triangular_Arbitrage_Binance.xlsx
@@ -1,36 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/eh1618_ic_ac_uk/Documents/Work/Fourth Year/Project/Research/crypto_arbitrage_bot/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_90F1685A710F0BAA5D7E528C73C0981495FC57C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4BF0D40-E3FA-46AA-8022-0DDFC0DE3DEB}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-28920" yWindow="8745" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Binance Timing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Binance" sheetId="1" r:id="rId1"/>
+    <sheet name="Binance Occ." sheetId="2" r:id="rId2"/>
+    <sheet name="Binance Timing" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="[hh]:mm:ss"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -48,84 +56,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -425,80 +371,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col width="18.26953125" customWidth="1" style="1" min="1" max="1"/>
-    <col width="20.26953125" customWidth="1" style="1" min="2" max="2"/>
-    <col width="19" customWidth="1" style="1" min="3" max="3"/>
-    <col width="22.453125" customWidth="1" style="1" min="4" max="4"/>
+    <col min="3" max="3" width="42.1796875" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>buy</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AUDUSDT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>LUNAAUD</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>LUNAUSDT</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.91838985784365</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>44693.6622156713</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>44693.66239370311</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>0.0001780318171296296</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>44693.66239580378</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>2.100671296296296e-06</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>